<commit_message>
update fixed reference file .xlsx
</commit_message>
<xml_diff>
--- a/doc/SDIO_reference.xlsx
+++ b/doc/SDIO_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -14,11 +14,10 @@
     <sheet name="IPIF_rel1.0.0" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="IPREGLIST_rel1.0.0" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="IPREGMAP_rel1.0.0" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="IPTREGMAP_rel1.0.0" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="IPUDMACMDLIST_rel1.0.0" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="IPUDMACMDMAP_rel1.0.0" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="IP_Program_Guide" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="IPTESTPLAN_rel1.0.0" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="IPUDMACMDLIST_rel1.0.0" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="IPUDMACMDMAP_rel1.0.0" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="IP_Program_Guide" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="IPTESTPLAN_rel1.0.0" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="IF_DIR" vbProcedure="false">#REF!</definedName>
@@ -28,13 +27,6 @@
     <definedName function="false" hidden="false" name="IF_TYPE" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="IF_VOLTAGE" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="REGISTERTYPE_LIST" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="IF_DIR" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="IF_IO" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="IF_ISO" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="IF_LVLSHIFT" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="IF_TYPE" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="IF_VOLTAGE" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="REGISTERTYPE_LIST" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -46,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="372">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -561,9 +553,6 @@
     <t xml:space="preserve">Register Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Header</t>
-  </si>
-  <si>
     <t xml:space="preserve">Address</t>
   </si>
   <si>
@@ -618,15 +607,6 @@
     <t xml:space="preserve">RX SDIO uDMA transfer configuration</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_RX_INITCFG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">SDIO_TX_SADDR</t>
   </si>
   <si>
@@ -652,12 +632,6 @@
   </si>
   <si>
     <t xml:space="preserve">TX SDIO uDMA transfer configuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_TX_INITCFG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x1C</t>
   </si>
   <si>
     <t xml:space="preserve">SDIO_CMD_OP</t>
@@ -945,18 +919,18 @@
   </si>
   <si>
     <t xml:space="preserve">Indicate the error status of the transfer of  command :
--6’b00000: no error
--6'b00001: Response Time Out
--6'b00010: Response Wrong Direction
--6'b00100: Response Busy Timeout</t>
+-6’b000000: no error
+-6'b000001: Response Time Out
+-6'b000010: Response Wrong Direction
+-6'b000100: Response Busy Timeout</t>
   </si>
   <si>
     <t xml:space="preserve">DATA_ERR_STATUS</t>
   </si>
   <si>
     <t xml:space="preserve">Indicate the error status of the transfer of  data :
--6’b00000: no error
--6'b00001: Response Time Out</t>
+-6’b000000: no error
+-6'b000001: Response Time Out</t>
   </si>
   <si>
     <t xml:space="preserve">STOPCMD_OP</t>
@@ -985,18 +959,18 @@
     <t xml:space="preserve">CLK_DIV</t>
   </si>
   <si>
-    <t xml:space="preserve">Clock diviser</t>
-  </si>
-  <si>
     <t xml:space="preserve">Command name</t>
   </si>
   <si>
-    <t xml:space="preserve">Command field</t>
+    <t xml:space="preserve">Command number</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
   <si>
+    <t xml:space="preserve">Parameter Size</t>
+  </si>
+  <si>
     <t xml:space="preserve">CMD_GO_IDLE_STATE</t>
   </si>
   <si>
@@ -1117,7 +1091,7 @@
     <t xml:space="preserve">STOP command for sd cards, stop multi block transfers after current block</t>
   </si>
   <si>
-    <t xml:space="preserve">Parameter bit field</t>
+    <t xml:space="preserve">Parameter Bit field</t>
   </si>
   <si>
     <t xml:space="preserve">Field value</t>
@@ -1127,21 +1101,6 @@
   </si>
   <si>
     <t xml:space="preserve">0x1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0X1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UDMA_GC-&gt;CG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x1A102000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOCEU-&gt;FC_MASK[8]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x1A106004 – 0x1A106024</t>
   </si>
   <si>
     <t xml:space="preserve">Operations</t>
@@ -1832,13 +1791,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1904,22 +1863,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="38.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,243 +2135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D23"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
-        <v>342</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="45"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="70" t="s">
-        <v>343</v>
-      </c>
-      <c r="C7" s="70" t="s">
-        <v>344</v>
-      </c>
-      <c r="D7" s="70" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="65" t="s">
-        <v>356</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>357</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>358</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="65" t="s">
-        <v>360</v>
-      </c>
-      <c r="B16" s="65" t="s">
-        <v>361</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>362</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-    </row>
-    <row r="18" customFormat="false" ht="158.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="65" t="s">
-        <v>363</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="C18" s="65" t="s">
-        <v>365</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="65" t="s">
-        <v>367</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>368</v>
-      </c>
-      <c r="C19" s="60" t="s">
-        <v>369</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="176.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="65" t="s">
-        <v>371</v>
-      </c>
-      <c r="B20" s="60" t="s">
-        <v>372</v>
-      </c>
-      <c r="C20" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="160.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="65" t="s">
-        <v>375</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>376</v>
-      </c>
-      <c r="C21" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="D21" s="55" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="65" t="s">
-        <v>377</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>378</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="65" t="s">
-        <v>379</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>380</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="D23" s="55" t="s">
-        <v>374</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:C6"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2422,20 +2145,19 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="42.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="42.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>11</v>
@@ -2446,30 +2168,29 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2810,7 +2531,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2820,14 +2541,13 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="43.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="44" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="44" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="44" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2891,28 +2611,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3658,28 +3374,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="36" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="36" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="46.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="36" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="36" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="4.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="25" width="46.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="36" width="9.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3690,10 +3407,10 @@
         <v>161</v>
       </c>
       <c r="C1" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="57" t="s">
         <v>162</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>78</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>163</v>
@@ -3704,542 +3421,547 @@
       <c r="G1" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="57" t="s">
         <v>166</v>
-      </c>
-      <c r="I1" s="58" t="s">
-        <v>11</v>
       </c>
       <c r="J1" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="57" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="36" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
+      <c r="B2" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>170</v>
-      </c>
-      <c r="D2" s="36" t="n">
-        <v>32</v>
       </c>
       <c r="E2" s="59" t="s">
         <v>171</v>
       </c>
       <c r="F2" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="G2" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H2" s="59" t="s">
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D3" s="59" t="s">
         <v>170</v>
-      </c>
-      <c r="I2" s="60" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="36" t="n">
-        <v>32</v>
       </c>
       <c r="E3" s="59" t="s">
         <v>171</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D4" s="59" t="s">
         <v>170</v>
-      </c>
-      <c r="I3" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" s="36" t="n">
-        <v>32</v>
       </c>
       <c r="E4" s="59" t="s">
         <v>171</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G4" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H4" s="59" t="s">
-        <v>175</v>
-      </c>
-      <c r="I4" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="J4" s="0"/>
-      <c r="K4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
+      <c r="B5" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="I5" s="59"/>
+      <c r="J5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="H5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="I5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
+      <c r="B6" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="59" t="s">
-        <v>184</v>
-      </c>
-      <c r="D6" s="36" t="n">
+      <c r="C6" s="36" t="n">
         <v>32</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>170</v>
       </c>
       <c r="E6" s="59" t="s">
         <v>171</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H6" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D7" s="59" t="s">
         <v>170</v>
-      </c>
-      <c r="I6" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="J6" s="0"/>
-      <c r="K6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="C7" s="59" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" s="36" t="n">
-        <v>32</v>
       </c>
       <c r="E7" s="59" t="s">
         <v>171</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D8" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="I7" s="60" t="s">
-        <v>188</v>
-      </c>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="C8" s="59" t="s">
+      <c r="E8" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="D8" s="36" t="n">
+      <c r="F8" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="36" t="n">
         <v>32</v>
       </c>
-      <c r="E8" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="F8" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="G8" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H8" s="59" t="s">
+      <c r="D9" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="I8" s="60" t="s">
+      <c r="E9" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>193</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="59" t="s">
-        <v>182</v>
-      </c>
       <c r="G9" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="H9" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="I9" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="J9" s="59"/>
-      <c r="K9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="C10" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="D10" s="36" t="n">
-        <v>14</v>
-      </c>
-      <c r="F10" s="59" t="s">
+      <c r="I9" s="59"/>
+      <c r="J9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>196</v>
       </c>
+      <c r="B10" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>190</v>
+      </c>
       <c r="G10" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="I10" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>198</v>
       </c>
+      <c r="I10" s="61"/>
       <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="B11" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="36" t="n">
+      <c r="C11" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F11" s="59" t="s">
-        <v>196</v>
+      <c r="D11" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>190</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="I11" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>201</v>
       </c>
+      <c r="I11" s="61"/>
       <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="B12" s="0"/>
-      <c r="C12" s="46" t="s">
+      <c r="B12" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="E12" s="0"/>
+      <c r="C12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>191</v>
+      </c>
       <c r="F12" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>204</v>
       </c>
+      <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="B13" s="0"/>
-      <c r="C13" s="46" t="s">
+      <c r="B13" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="0"/>
+      <c r="C13" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>191</v>
+      </c>
       <c r="F13" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="G13" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>207</v>
       </c>
+      <c r="I13" s="61"/>
       <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="0"/>
-      <c r="C14" s="46" t="s">
+      <c r="B14" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="C14" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E14" s="0"/>
+      <c r="D14" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>191</v>
+      </c>
       <c r="F14" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="G14" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="H14" s="0"/>
-      <c r="I14" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="0"/>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="C15" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E15" s="0"/>
+      <c r="D15" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>191</v>
+      </c>
       <c r="F15" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="G15" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="H15" s="0"/>
-      <c r="I15" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="B16" s="0"/>
-      <c r="C16" s="46" t="s">
+      <c r="B16" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="C16" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E16" s="0"/>
+      <c r="D16" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>171</v>
+      </c>
       <c r="F16" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="G16" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="H16" s="0"/>
-      <c r="I16" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>216</v>
       </c>
+      <c r="I16" s="0"/>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
       <c r="L16" s="0"/>
-      <c r="M16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B17" s="0"/>
-      <c r="C17" s="46" t="s">
+      <c r="B17" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="C17" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E17" s="0"/>
+      <c r="D17" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>171</v>
+      </c>
       <c r="F17" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="G17" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="H17" s="0"/>
-      <c r="I17" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>219</v>
       </c>
+      <c r="I17" s="0"/>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
       <c r="L17" s="0"/>
-      <c r="M17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B18" s="0"/>
-      <c r="C18" s="46" t="s">
+      <c r="B18" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E18" s="0"/>
-      <c r="F18" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="G18" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0" t="s">
+      <c r="C18" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>222</v>
       </c>
+      <c r="I18" s="0"/>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
       <c r="L18" s="0"/>
-      <c r="M18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="0"/>
-      <c r="C19" s="46" t="s">
+      <c r="B19" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E19" s="0"/>
-      <c r="F19" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0" t="s">
+      <c r="C19" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="25" t="s">
         <v>225</v>
       </c>
+      <c r="I19" s="0"/>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
       <c r="L19" s="0"/>
-      <c r="M19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>227</v>
-      </c>
-      <c r="D20" s="36" t="n">
-        <v>14</v>
-      </c>
-      <c r="F20" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="G20" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>228</v>
-      </c>
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="C21" s="59" t="s">
-        <v>230</v>
-      </c>
-      <c r="D21" s="36" t="n">
-        <v>32</v>
-      </c>
-      <c r="F21" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="G21" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1" type="list">
       <formula1>REGISTERTYPE_LIST</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4255,49 +3977,49 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="73.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="63" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="63" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
       </c>
       <c r="E1" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="45" t="s">
         <v>164</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>165</v>
       </c>
       <c r="G1" s="45" t="s">
         <v>79</v>
@@ -4308,10 +4030,10 @@
     </row>
     <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="44" t="n">
         <v>0</v>
@@ -4320,24 +4042,24 @@
         <v>32</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G2" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="65" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="44" t="n">
         <v>0</v>
@@ -4346,24 +4068,24 @@
         <v>20</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G3" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H3" s="67" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="44" t="n">
         <v>0</v>
@@ -4372,24 +4094,24 @@
         <v>1</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G4" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="44" t="n">
         <v>1</v>
@@ -4398,24 +4120,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="44" t="n">
         <v>4</v>
@@ -4424,24 +4146,24 @@
         <v>1</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G6" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H6" s="67" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="44" t="n">
         <v>6</v>
@@ -4450,24 +4172,24 @@
         <v>1</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G7" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H7" s="67" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="44" t="n">
         <v>5</v>
@@ -4476,464 +4198,464 @@
         <v>1</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G8" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H8" s="67" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46" t="s">
-        <v>182</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="65" t="s">
+        <v>244</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="H9" s="59" t="s">
-        <v>182</v>
+        <v>179</v>
+      </c>
+      <c r="C9" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="44" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" s="44" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="44" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F10" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="44" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="44" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G11" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H11" s="67" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="65" t="s">
+      <c r="B13" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="44" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="67" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="C12" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H12" s="67" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="65" t="s">
-        <v>241</v>
-      </c>
-      <c r="B13" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="C13" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="G13" s="66" t="s">
-        <v>242</v>
-      </c>
-      <c r="H13" s="67" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="65" t="s">
-        <v>244</v>
-      </c>
       <c r="B14" s="59" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C14" s="44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14" s="44" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="F14" s="44" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="G14" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H14" s="67" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B15" s="59" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C15" s="44" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="44" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G15" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H15" s="67" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="67" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="65" t="s">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="B16" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="44" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="G16" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H16" s="67" t="s">
+      <c r="B17" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="67" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="B17" s="59" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="F17" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" s="59" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C18" s="44" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="44" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E18" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="67" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="65" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="C19" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="67" t="s">
+        <v>253</v>
+      </c>
+      <c r="J19" s="67"/>
+    </row>
+    <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H18" s="67" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="65" t="s">
-        <v>254</v>
-      </c>
-      <c r="B19" s="59" t="s">
-        <v>194</v>
-      </c>
-      <c r="C19" s="44" t="n">
-        <v>8</v>
-      </c>
-      <c r="D19" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="E19" s="59" t="s">
+      <c r="C20" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" s="67" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="F19" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="G19" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H19" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="J19" s="67"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="65" t="s">
-        <v>256</v>
-      </c>
-      <c r="B20" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="C20" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="44" t="n">
-        <v>32</v>
-      </c>
-      <c r="E20" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F20" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H20" s="67" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="65" t="s">
-        <v>258</v>
-      </c>
-      <c r="B21" s="59" t="s">
-        <v>202</v>
-      </c>
       <c r="C21" s="44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" s="44" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H21" s="67" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="65" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="C22" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D22" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="E22" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H22" s="67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="65" t="s">
+        <v>260</v>
+      </c>
+      <c r="B23" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="G21" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H21" s="67" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="65" t="s">
-        <v>260</v>
-      </c>
-      <c r="B22" s="59" t="s">
+      <c r="C23" s="46" t="n">
+        <v>16</v>
+      </c>
+      <c r="D23" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="H23" s="60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F22" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="G22" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H22" s="67" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="65" t="s">
-        <v>262</v>
-      </c>
-      <c r="B23" s="59" t="s">
+      <c r="B25" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="G23" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H23" s="67" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="65" t="s">
+      <c r="C25" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="46" t="n">
+        <v>32</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="H25" s="60" t="s">
         <v>264</v>
       </c>
-      <c r="B24" s="59" t="s">
-        <v>202</v>
-      </c>
-      <c r="C24" s="44" t="n">
-        <v>8</v>
-      </c>
-      <c r="D24" s="44" t="n">
-        <v>8</v>
-      </c>
-      <c r="E24" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="G24" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H24" s="67" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="65" t="s">
-        <v>266</v>
-      </c>
-      <c r="B25" s="59" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="46" t="n">
-        <v>16</v>
-      </c>
-      <c r="D25" s="46" t="n">
-        <v>10</v>
-      </c>
-      <c r="E25" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F25" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="G25" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="H25" s="60" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="65" t="s">
-        <v>268</v>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>205</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>205</v>
@@ -4942,22 +4664,22 @@
         <v>0</v>
       </c>
       <c r="D26" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F26" s="59" t="s">
-        <v>196</v>
+        <v>32</v>
+      </c>
+      <c r="E26" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="66" t="s">
+        <v>191</v>
       </c>
       <c r="G26" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H26" s="60" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>208</v>
       </c>
@@ -4971,16 +4693,16 @@
         <v>32</v>
       </c>
       <c r="E27" s="66" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F27" s="66" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G27" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H27" s="60" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4997,277 +4719,245 @@
         <v>32</v>
       </c>
       <c r="E28" s="66" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F28" s="66" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G28" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H28" s="60" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C29" s="46" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="46" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E29" s="66" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="F29" s="66" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="G29" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H29" s="60" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>217</v>
       </c>
       <c r="C30" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="46" t="n">
+        <v>16</v>
+      </c>
+      <c r="D31" s="46" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="H31" s="60" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="44" t="n">
+        <v>24</v>
+      </c>
+      <c r="D32" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="H32" s="60" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D33" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F33" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H33" s="67" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="65" t="s">
+        <v>278</v>
+      </c>
+      <c r="B34" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="44" t="n">
         <v>0</v>
       </c>
-      <c r="D30" s="46" t="n">
+      <c r="D34" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="G34" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" s="67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C35" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="44" t="n">
         <v>32</v>
       </c>
-      <c r="E30" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="F30" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="G30" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="H30" s="60" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="C31" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="66" t="s">
-        <v>172</v>
-      </c>
-      <c r="F31" s="66" t="s">
-        <v>172</v>
-      </c>
-      <c r="G31" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="H31" s="60" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B32" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="C32" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="H32" s="60" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="C33" s="46" t="n">
-        <v>16</v>
-      </c>
-      <c r="D33" s="46" t="n">
-        <v>6</v>
-      </c>
-      <c r="E33" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="G33" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="H33" s="60" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B34" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="C34" s="44" t="n">
-        <v>24</v>
-      </c>
-      <c r="D34" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="G34" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="H34" s="60" t="s">
+      <c r="E35" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G35" s="66" t="s">
+        <v>169</v>
+      </c>
+      <c r="H35" s="67" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="35" t="s">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="B35" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="C35" s="44" t="n">
-        <v>8</v>
-      </c>
-      <c r="D35" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F35" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="G35" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H35" s="67" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="65" t="s">
-        <v>284</v>
-      </c>
       <c r="B36" s="46" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C36" s="44" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="44" t="n">
-        <v>3</v>
-      </c>
-      <c r="E36" s="59" t="s">
-        <v>196</v>
+        <v>9</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>190</v>
       </c>
       <c r="F36" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="G36" s="66" t="s">
-        <v>170</v>
+        <v>191</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>169</v>
       </c>
       <c r="H36" s="67" t="s">
-        <v>285</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="35" t="s">
-        <v>286</v>
-      </c>
-      <c r="B37" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="C37" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" s="44" t="n">
-        <v>32</v>
-      </c>
-      <c r="E37" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F37" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="G37" s="66" t="s">
-        <v>170</v>
-      </c>
-      <c r="H37" s="67" t="s">
-        <v>287</v>
-      </c>
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="35" t="s">
-        <v>288</v>
-      </c>
-      <c r="B38" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="44" t="n">
-        <v>9</v>
-      </c>
-      <c r="E38" s="44" t="s">
-        <v>196</v>
-      </c>
-      <c r="F38" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="G38" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="H38" s="62" t="s">
-        <v>289</v>
-      </c>
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -5282,374 +4972,314 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="63" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="63" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="16.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="30.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="63" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="38.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="76.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="76.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="68" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>233</v>
+        <v>283</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>78</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>78</v>
+        <v>285</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="F1" s="68" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="55" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>293</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B8" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>311</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B10" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B12" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="44" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="76.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.37"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>291</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>292</v>
-      </c>
-      <c r="E1" s="68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="B2" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55" t="s">
-        <v>296</v>
-      </c>
-      <c r="B3" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>242</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="B4" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>299</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="B5" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B6" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="B7" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>309</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>310</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="B8" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>313</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="B9" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>316</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="B10" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>320</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="B11" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="B12" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>200</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="B13" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>328</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="B14" s="44" t="n">
-        <v>6</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>331</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>294</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F28"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="76.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="F1" s="68" t="s">
         <v>11</v>
@@ -5657,10 +5287,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C2" s="44" t="n">
         <v>8</v>
@@ -5669,15 +5299,15 @@
         <v>6</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C3" s="44" t="n">
         <v>0</v>
@@ -5686,15 +5316,15 @@
         <v>3</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C4" s="44" t="n">
         <v>8</v>
@@ -5703,15 +5333,15 @@
         <v>6</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C5" s="44" t="n">
         <v>0</v>
@@ -5720,15 +5350,15 @@
         <v>3</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C6" s="44" t="n">
         <v>8</v>
@@ -5737,15 +5367,15 @@
         <v>6</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C7" s="44" t="n">
         <v>0</v>
@@ -5754,15 +5384,15 @@
         <v>3</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C8" s="44" t="n">
         <v>8</v>
@@ -5771,15 +5401,15 @@
         <v>6</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C9" s="44" t="n">
         <v>0</v>
@@ -5788,15 +5418,15 @@
         <v>3</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C10" s="44" t="n">
         <v>8</v>
@@ -5805,15 +5435,15 @@
         <v>6</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C11" s="44" t="n">
         <v>0</v>
@@ -5822,15 +5452,15 @@
         <v>3</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C12" s="44" t="n">
         <v>8</v>
@@ -5839,15 +5469,15 @@
         <v>6</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C13" s="44" t="n">
         <v>0</v>
@@ -5856,15 +5486,15 @@
         <v>3</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C14" s="44" t="n">
         <v>8</v>
@@ -5873,15 +5503,15 @@
         <v>6</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C15" s="44" t="n">
         <v>0</v>
@@ -5890,15 +5520,15 @@
         <v>3</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C16" s="44" t="n">
         <v>8</v>
@@ -5907,15 +5537,15 @@
         <v>6</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C17" s="44" t="n">
         <v>0</v>
@@ -5924,15 +5554,15 @@
         <v>3</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C18" s="44" t="n">
         <v>8</v>
@@ -5941,15 +5571,15 @@
         <v>6</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C19" s="44" t="n">
         <v>0</v>
@@ -5958,15 +5588,15 @@
         <v>3</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C20" s="44" t="n">
         <v>8</v>
@@ -5975,15 +5605,15 @@
         <v>6</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C21" s="44" t="n">
         <v>0</v>
@@ -5992,15 +5622,15 @@
         <v>3</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C22" s="44" t="n">
         <v>8</v>
@@ -6009,15 +5639,15 @@
         <v>6</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C23" s="44" t="n">
         <v>0</v>
@@ -6026,15 +5656,15 @@
         <v>3</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C24" s="44" t="n">
         <v>8</v>
@@ -6043,15 +5673,15 @@
         <v>6</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C25" s="44" t="n">
         <v>0</v>
@@ -6060,15 +5690,15 @@
         <v>3</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="65" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C26" s="44" t="n">
         <v>8</v>
@@ -6077,15 +5707,15 @@
         <v>6</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C27" s="44" t="n">
         <v>0</v>
@@ -6094,7 +5724,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6104,8 +5734,284 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D78"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="70" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="65" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>346</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="65" t="s">
+        <v>349</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>350</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+    </row>
+    <row r="13" customFormat="false" ht="158.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>353</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>354</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="176.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65" t="s">
+        <v>360</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>361</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="160.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="s">
+        <v>364</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65" t="s">
+        <v>366</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>367</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>